<commit_message>
Exibir postagens e imagens corretas na Home
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -197,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +216,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -229,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -239,6 +245,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,7 +780,7 @@
       <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -785,7 +792,7 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -797,7 +804,7 @@
       <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">

</xml_diff>

<commit_message>
Exibir imagens na Home e na Home Preview
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t>Bug</t>
   </si>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,7 +804,7 @@
       <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -816,19 +816,19 @@
       <c r="C23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -840,7 +840,7 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -949,6 +949,18 @@
         <v>4</v>
       </c>
       <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementação da funcionalidade 'Search'
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -197,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,12 +216,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -235,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -245,7 +239,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +522,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -840,7 +833,7 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
Criado funcionalidade para inserir texto da política de privacidade
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
   <si>
     <t>Bug</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Home Preview</t>
+  </si>
+  <si>
+    <t>Atualizar para CKEditor formulários de textos fixos no site</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -845,7 +848,7 @@
       <c r="C26" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -857,7 +860,7 @@
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -954,6 +957,18 @@
         <v>4</v>
       </c>
       <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajustes do destaque do menu
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -549,7 +549,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -968,7 +968,7 @@
       <c r="C34" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">

</xml_diff>

<commit_message>
Inserção de ícones no menu
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
   <si>
     <t>Bug</t>
   </si>
@@ -200,7 +200,28 @@
     <t>Ao clicar em "Leia Mais", redirecionar o usuário para a busca sobre aquele lugar</t>
   </si>
   <si>
-    <t>Ao aplicar aterações, não deve alterar images que não estejam selecionadas</t>
+    <t>Testes de segurança</t>
+  </si>
+  <si>
+    <t>Testes</t>
+  </si>
+  <si>
+    <t>Ao aplicar alterações, não deve alterar imagens que não estejam selecionadas</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Verificar mensagem de erro que acontece após fazer o login</t>
+  </si>
+  <si>
+    <t>Analisar a possibilidade de inserir ícones quando for postar algo</t>
+  </si>
+  <si>
+    <t>Postar</t>
+  </si>
+  <si>
+    <t>Ajustar tamanho dos botões no mobile</t>
   </si>
 </sst>
 </file>
@@ -224,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +264,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -256,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -266,6 +293,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -975,12 +1003,12 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -992,67 +1020,115 @@
       <c r="C36" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
         <v>54</v>
       </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="3"/>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>